<commit_message>
bug fixing on Warning when IfCondMismatch
</commit_message>
<xml_diff>
--- a/2-Tests/Lexerow.Core.Tests/10-Files/OnExcelIfInStringItemsOk.xlsx
+++ b/2-Tests/Lexerow.Core.Tests/10-Files/OnExcelIfInStringItemsOk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a990f455bb745add/ProjetsDev/10-Pierlam/Lexerow/Dev/Lexerow/2-Tests/Lexerow.Core.Tests/10-Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="11_E721A496124379684413B01EE7A22F2143A1BA3B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B4AC4B6-3A0F-4D5F-B50E-8623E0B3D673}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_E721A496124379684413B01EE7A22F2143A1BA3B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DB91A55-C940-4CCF-806C-55C45D72C007}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="5130" windowWidth="17535" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>action</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>type is int not string</t>
+  </si>
+  <si>
+    <t>blabla</t>
   </si>
 </sst>
 </file>
@@ -121,6 +127,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -386,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,6 +473,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>